<commit_message>
Excel actualizado. Eliminacion de codigo conflictivo en generacion de señal
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tengo miedo\4 Grado\FSI\Sonido\ProyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366AAA5E-3F15-4532-BE97-A7F1DA49BA7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C53878-664D-4F51-B0E2-EFBE48E5B707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -145,13 +145,19 @@
   </si>
   <si>
     <t>Número</t>
+  </si>
+  <si>
+    <t>Juero que se ha puesto asi solo. Att Jennifer.</t>
+  </si>
+  <si>
+    <t>Dudo que se implemente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +187,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +239,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -459,11 +478,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -502,6 +537,60 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -520,15 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -538,53 +618,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -897,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
-  <dimension ref="B1:J37"/>
+  <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,19 +952,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="9" t="s">
         <v>16</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -936,17 +982,17 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
@@ -955,515 +1001,519 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="36">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35">
+      <c r="B7" s="16">
         <v>2</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35">
+      <c r="B8" s="16">
         <v>3</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+      <c r="B9" s="30">
         <v>4</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="29" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="31"/>
+      <c r="J9" s="28"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="32"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35">
+      <c r="B11" s="16">
         <v>5</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="33">
+      <c r="B12" s="30">
         <v>6</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="29" t="s">
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="34"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="15"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="35">
+      <c r="B14" s="16">
         <v>7</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="35">
+      <c r="B15" s="16">
         <v>8</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
       <c r="I15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35">
+      <c r="B16" s="16">
         <v>9</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
       <c r="I16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+    <row r="17" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="16">
         <v>10</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
       <c r="I17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="2:12" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="16">
         <v>11</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="35">
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="2:12" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16">
         <v>12</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="22"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
       <c r="I19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35">
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="16">
         <v>13</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
       <c r="I20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="2:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35">
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="16">
         <v>14</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="22"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
       <c r="I21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35">
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
         <v>15</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="22"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="35">
+    <row r="23" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
         <v>16</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
       <c r="I23" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="35">
+    <row r="24" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
         <v>17</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
       <c r="I24" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="35">
+    <row r="25" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
         <v>18</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="27"/>
       <c r="I25" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="35">
+    <row r="26" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
         <v>19</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="27"/>
       <c r="I26" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="35">
+    <row r="27" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
         <v>20</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
       <c r="I27" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35">
+    <row r="28" spans="2:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="16">
         <v>21</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
       <c r="I28" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="35">
+    <row r="29" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="16">
         <v>22</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="22"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="27"/>
       <c r="I29" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="35">
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="16">
         <v>23</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="35">
+    <row r="31" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="16">
         <v>24</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="27"/>
       <c r="I31" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="35">
+    <row r="32" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="16">
         <v>25</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
       <c r="I32" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="35">
+      <c r="B33" s="16">
         <v>26</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="22"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="27"/>
       <c r="I33" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="35">
+      <c r="B34" s="16">
         <v>27</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="22"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="27"/>
       <c r="I34" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="35">
+      <c r="B35" s="16">
         <v>28</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="22"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="35">
+      <c r="B36" s="16">
         <v>29</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="22"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="27"/>
       <c r="I36" s="13" t="s">
         <v>30</v>
       </c>
@@ -1471,13 +1521,26 @@
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
+  <mergeCells count="38">
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C9:H10"/>
+    <mergeCell ref="C12:H13"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
     <mergeCell ref="C22:H22"/>
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C14:H14"/>
@@ -1488,27 +1551,15 @@
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C20:H20"/>
     <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="J12:J13"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C35:H35"/>
-    <mergeCell ref="C36:H36"/>
-    <mergeCell ref="C9:H10"/>
-    <mergeCell ref="C12:H13"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="C23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
cambio en el documento
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tengo miedo\4 Grado\FSI\Sonido\ProyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C53878-664D-4F51-B0E2-EFBE48E5B707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F79152-0045-4181-A08F-121E822C8C73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Número</t>
-  </si>
-  <si>
-    <t>Juero que se ha puesto asi solo. Att Jennifer.</t>
   </si>
   <si>
     <t>Dudo que se implemente</t>
@@ -157,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +188,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -493,12 +498,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -537,12 +553,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -552,6 +562,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -568,15 +612,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,34 +632,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -940,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
-  <dimension ref="B1:L37"/>
+  <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,15 +989,15 @@
       <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="37"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="43" t="s">
-        <v>41</v>
+      <c r="J2" s="18" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -982,17 +1012,17 @@
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1001,519 +1031,516 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>2</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>3</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30">
+      <c r="B9" s="37">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="28"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="21"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="42"/>
-      <c r="J10" s="29"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <v>5</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30">
+      <c r="B12" s="37">
         <v>6</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="32"/>
+      <c r="J12" s="39"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="42"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
+      <c r="B14" s="14">
         <v>7</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="27"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
+      <c r="B15" s="14">
         <v>8</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
+      <c r="B16" s="14">
         <v>9</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="27"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
       <c r="I16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="2:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="16">
+    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="14">
         <v>10</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="2:12" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16">
+      <c r="J17" s="48"/>
+    </row>
+    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="14">
         <v>11</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="11" t="s">
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="43"/>
-    </row>
-    <row r="19" spans="2:12" ht="23.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="16">
+      <c r="J18" s="49"/>
+    </row>
+    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="14">
         <v>12</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="27"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="25"/>
       <c r="I19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="16">
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="14">
         <v>13</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="16">
+      <c r="J20" s="44"/>
+      <c r="K20" s="47"/>
+    </row>
+    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14">
         <v>14</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="11" t="s">
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16">
+      <c r="J21" s="46"/>
+    </row>
+    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14">
         <v>15</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="27"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
+      <c r="J22" s="45"/>
+    </row>
+    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="14">
         <v>16</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="16">
+    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14">
         <v>17</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
+    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14">
         <v>18</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
+    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14">
         <v>19</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="27"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
+    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="14">
         <v>20</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="27"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="2:12" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+    <row r="28" spans="2:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="14">
         <v>21</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="27"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16">
+    <row r="29" spans="2:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="14">
         <v>22</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="27"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="25"/>
       <c r="I29" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="16">
+    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="14">
         <v>23</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="27"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="16">
+    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="14">
         <v>24</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="16">
+    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="14">
         <v>25</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="27"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="25"/>
       <c r="I32" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="16">
+      <c r="B33" s="14">
         <v>26</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="27"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="25"/>
       <c r="I33" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="16">
+      <c r="B34" s="14">
         <v>27</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="27"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="25"/>
       <c r="I34" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="16">
+      <c r="B35" s="14">
         <v>28</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="25"/>
       <c r="I35" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="16">
+      <c r="B36" s="14">
         <v>29</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="27"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="25"/>
       <c r="I36" s="13" t="s">
         <v>30</v>
       </c>
@@ -1521,8 +1548,29 @@
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="J20:K20"/>
+  <mergeCells count="37">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1538,28 +1586,6 @@
     <mergeCell ref="C23:H23"/>
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ultimo push de funcionalidades
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Escritorio\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F9B23B-E9A3-4CEE-9755-A0258DB87699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CD33C5-B315-4F06-B4A1-B5058D40C6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -517,11 +517,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -529,12 +526,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,9 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -565,27 +553,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,15 +616,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,35 +642,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -984,593 +980,614 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="10" width="19.44140625" customWidth="1"/>
+    <col min="9" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="7" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16" t="s">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="2" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15">
+    <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="10" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14">
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="10" t="s">
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14">
+      <c r="J7" s="18"/>
+    </row>
+    <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="10" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="37">
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="38">
         <v>4</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="41" t="s">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="35"/>
-    </row>
-    <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="36"/>
-    </row>
-    <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14">
+      <c r="J9" s="36"/>
+    </row>
+    <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="39"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="10" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="37">
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="38">
         <v>6</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="41" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="39"/>
-    </row>
-    <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="40"/>
-    </row>
-    <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14">
+      <c r="J12" s="40"/>
+    </row>
+    <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="39"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="41"/>
+    </row>
+    <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="10" t="s">
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="10" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14">
+    <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="10" t="s">
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14">
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="11" t="s">
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="24"/>
-    </row>
-    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14">
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="20" t="s">
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="25"/>
-    </row>
-    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14">
+      <c r="J18" s="44"/>
+    </row>
+    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="11" t="s">
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14">
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="11" t="s">
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="23"/>
-    </row>
-    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14">
+      <c r="J20" s="15"/>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="20" t="s">
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14">
+      <c r="J21" s="45"/>
+    </row>
+    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="11" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="J22" s="46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14">
+    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="11" t="s">
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14">
+      <c r="J23" s="47"/>
+    </row>
+    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="11" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="51" t="s">
+      <c r="J24" s="48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="14">
+    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="11" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14">
+      <c r="J25" s="50"/>
+    </row>
+    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="11" t="s">
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="14">
+      <c r="J26" s="50"/>
+    </row>
+    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="11" t="s">
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="14">
+      <c r="J27" s="50"/>
+    </row>
+    <row r="28" spans="2:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="11" t="s">
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="14">
+      <c r="J28" s="50"/>
+    </row>
+    <row r="29" spans="2:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="13" t="s">
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="50" t="s">
+      <c r="J29" s="49" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="14">
+    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="13" t="s">
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14">
+      <c r="J30" s="50"/>
+    </row>
+    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="13" t="s">
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14">
+      <c r="J31" s="50"/>
+    </row>
+    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="13" t="s">
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="51" t="s">
+      <c r="J32" s="48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14">
+    <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="13" t="s">
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="14">
+      <c r="J33" s="50"/>
+    </row>
+    <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="13" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="14">
+      <c r="J34" s="50"/>
+    </row>
+    <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="13" t="s">
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="14">
+      <c r="J35" s="50"/>
+    </row>
+    <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="13" t="s">
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="J36" s="50"/>
+    </row>
+    <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1587,27 +1604,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
boton de espectrograma aun no funcional
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CD33C5-B315-4F06-B4A1-B5058D40C6BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FC9D7-DAB8-4CC2-94AE-18319A594E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
   </bookViews>
@@ -517,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -570,6 +570,75 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -582,15 +651,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -600,67 +660,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,10 +1009,10 @@
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="46"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1023,14 +1035,14 @@
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1042,14 +1054,14 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1059,14 +1071,14 @@
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1076,104 +1088,104 @@
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="18"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38">
+      <c r="B9" s="37">
         <v>4</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="42" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="38">
+      <c r="B12" s="37">
         <v>6</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="42" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="40"/>
+      <c r="J12" s="39"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="41"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1183,14 +1195,14 @@
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
@@ -1202,14 +1214,14 @@
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
@@ -1219,14 +1231,14 @@
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1236,48 +1248,48 @@
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="44"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="54"/>
     </row>
     <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="26"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1288,35 +1300,35 @@
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="26"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="45"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="26"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="46" t="s">
+      <c r="J22" s="22" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1324,35 +1336,35 @@
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="26"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="47"/>
+      <c r="J23" s="23"/>
     </row>
     <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="34"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="48" t="s">
+      <c r="J24" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1360,86 +1372,86 @@
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="26"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="34"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="50"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="26"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="50"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="50"/>
-    </row>
-    <row r="28" spans="2:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="25"/>
+    </row>
+    <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="26"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="34"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="50"/>
-    </row>
-    <row r="29" spans="2:11" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="51"/>
+    </row>
+    <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="9" t="s">
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="49" t="s">
+      <c r="J29" s="53" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1447,52 +1459,52 @@
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="26"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="34"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="50"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="26"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="34"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="50"/>
+      <c r="J31" s="25"/>
     </row>
     <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="26"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="48" t="s">
+      <c r="J32" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1500,94 +1512,73 @@
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="26"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="50"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="26"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="34"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="50"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="26"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="34"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="50"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="26"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="50"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1604,6 +1595,27 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Boton de combinar casi funcional y añadida robustez genérica
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2FC9D7-DAB8-4CC2-94AE-18319A594E6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79A0711-9262-405D-A0B6-ADF3D8A91ED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
   </bookViews>
@@ -588,6 +588,51 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -604,15 +649,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,42 +673,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,10 +1009,10 @@
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="46"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1035,14 +1035,14 @@
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1054,14 +1054,14 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1071,14 +1071,14 @@
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="46"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1088,104 +1088,104 @@
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="18"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37">
+      <c r="B9" s="49">
         <v>4</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="41" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="35"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="48"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="37">
+      <c r="B12" s="49">
         <v>6</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="41" t="s">
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="39"/>
+      <c r="J12" s="51"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="40"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="52"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1195,14 +1195,14 @@
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
@@ -1214,14 +1214,14 @@
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
@@ -1231,14 +1231,14 @@
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1248,14 +1248,14 @@
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="14" t="s">
         <v>17</v>
       </c>
@@ -1265,31 +1265,31 @@
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="54"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1300,14 +1300,14 @@
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="14" t="s">
         <v>17</v>
       </c>
@@ -1317,14 +1317,14 @@
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
@@ -1336,14 +1336,14 @@
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="34"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
@@ -1353,14 +1353,14 @@
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
@@ -1372,14 +1372,14 @@
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
@@ -1389,14 +1389,14 @@
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="34"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
@@ -1406,14 +1406,14 @@
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
@@ -1423,35 +1423,35 @@
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="51"/>
+      <c r="J28" s="27"/>
     </row>
     <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="50" t="s">
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="53" t="s">
+      <c r="J29" s="29" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1459,31 +1459,31 @@
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="52"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
@@ -1493,14 +1493,14 @@
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
@@ -1512,14 +1512,14 @@
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
@@ -1529,31 +1529,31 @@
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="25"/>
+      <c r="J34" s="24"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
@@ -1563,14 +1563,14 @@
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
@@ -1579,6 +1579,27 @@
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1595,27 +1616,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Añadido espectrograma y algunos bugs eliminados
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79A0711-9262-405D-A0B6-ADF3D8A91ED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC116C63-D274-4542-AF9D-3B8E17FF41EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>David</t>
+  </si>
+  <si>
+    <t>Casi</t>
   </si>
 </sst>
 </file>
@@ -517,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -557,9 +560,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -600,7 +600,52 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -615,15 +660,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -631,48 +667,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -992,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,10 +1003,10 @@
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="48"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1035,14 +1029,14 @@
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1054,159 +1048,159 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="18"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="46"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="18"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="18"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="49">
+      <c r="B9" s="41">
         <v>4</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="53" t="s">
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="47"/>
+      <c r="J9" s="39"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="50"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="48"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="18"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="49">
+      <c r="B12" s="41">
         <v>6</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="53" t="s">
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="51"/>
+      <c r="J12" s="39"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="50"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="52"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1214,121 +1208,123 @@
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="17"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="38"/>
       <c r="I18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="20"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="30"/>
+      <c r="J19" s="29" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="38"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="15"/>
-      <c r="K20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="38"/>
       <c r="I21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="21"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="38"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="21" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1336,35 +1332,35 @@
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="23"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="38"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="J24" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1372,86 +1368,86 @@
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="38"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="25"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="25"/>
+      <c r="J26" s="24"/>
     </row>
     <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="25"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="27"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="26" t="s">
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="29" t="s">
+      <c r="J29" s="28" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1459,52 +1455,52 @@
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="28"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="25"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="24" t="s">
+      <c r="J32" s="23" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1512,94 +1508,75 @@
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="25"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="24"/>
+      <c r="J34" s="23" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="38"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="25"/>
+      <c r="J35" s="24"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="25"/>
+      <c r="J36" s="24"/>
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1616,6 +1593,27 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modulacion implementada, a cambiar plots
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Escritorio\FSI\Sonido\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\OneDrive\Escritorio\sony\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6516D7F-8820-4E67-BF95-A72F27E05BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BADA7F75-6ADA-4298-8549-C53FE05F4924}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -159,7 +158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -526,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -573,9 +572,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -609,6 +605,57 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -621,15 +668,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,43 +677,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -992,30 +997,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21D07B-C296-4548-AFCC-8D5E95E61731}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="10" width="19.44140625" customWidth="1"/>
+    <col min="9" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="33"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1023,7 +1028,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1034,18 +1039,18 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1053,560 +1058,539 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="45"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="48">
+    <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="42">
         <v>4</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="50" t="s">
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="46"/>
-    </row>
-    <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="49"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="47"/>
-    </row>
-    <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="40"/>
+    </row>
+    <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="43"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="41"/>
+    </row>
+    <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="48">
+    <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="42">
         <v>6</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="50" t="s">
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="46"/>
-    </row>
-    <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="49"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="47"/>
-    </row>
-    <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="53"/>
+    </row>
+    <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="43"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="54"/>
+    </row>
+    <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="17"/>
     </row>
-    <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="J17" s="16"/>
     </row>
-    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
       <c r="I18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="19"/>
-    </row>
-    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
       <c r="J20" s="16"/>
       <c r="K20" s="15"/>
     </row>
-    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
       <c r="I21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="39"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="22"/>
-    </row>
-    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="36"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="39"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="24"/>
-    </row>
-    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="39"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="24"/>
-    </row>
-    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="36"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="39"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="24"/>
-    </row>
-    <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="23"/>
+    </row>
+    <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="36"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="26"/>
-    </row>
-    <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="25"/>
+    </row>
+    <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="25" t="s">
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="28" t="s">
+      <c r="J29" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="36"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="27"/>
-    </row>
-    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="36"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="24"/>
-    </row>
-    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="23"/>
+    </row>
+    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="23" t="s">
+      <c r="J32" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="36"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="24"/>
-    </row>
-    <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="23"/>
+    </row>
+    <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="36"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="J34" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="36"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="39"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J35" s="23"/>
+    </row>
+    <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="39"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="24"/>
-    </row>
-    <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="J36" s="23"/>
+    </row>
+    <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1623,6 +1607,27 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
boton combinar, cuantificacion asegurada, cambiados nombres y boton de reset
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\OneDrive\Escritorio\sony\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA4352C-50C1-4E7C-AF35-9140F4B3B8EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -146,19 +147,13 @@
     <t>Número</t>
   </si>
   <si>
-    <t>Dudo que se implemente</t>
-  </si>
-  <si>
     <t>David</t>
-  </si>
-  <si>
-    <t>Casi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -206,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,12 +249,6 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -525,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -561,7 +550,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,13 +590,40 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -627,15 +642,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -650,37 +656,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -997,11 +982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,22 +995,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="49"/>
+      <c r="H2" s="32"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1043,14 +1025,14 @@
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="48"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1062,535 +1044,550 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="17"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="17"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="17"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42">
+      <c r="B9" s="47">
         <v>4</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="44" t="s">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="40"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="41"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="17"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="42">
+      <c r="B12" s="47">
         <v>6</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="44" t="s">
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="53"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="54"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="50"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="17"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="30" t="s">
-        <v>41</v>
-      </c>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="29"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="16"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="14" t="s">
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="18"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="16"/>
-      <c r="K20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="14" t="s">
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="19"/>
+      <c r="J21" s="18"/>
     </row>
     <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="20" t="s">
-        <v>41</v>
+      <c r="J22" s="19" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="39"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="21"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="39"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="22" t="s">
-        <v>41</v>
+      <c r="J24" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="39"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="21"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="21"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="23"/>
+      <c r="J27" s="22"/>
     </row>
     <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="25"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="24" t="s">
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="27" t="s">
-        <v>41</v>
+      <c r="J29" s="26" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="39"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="35"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="26"/>
+      <c r="J30" s="25"/>
     </row>
     <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="39"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="35"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="23"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="39"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="22" t="s">
-        <v>41</v>
+      <c r="J32" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="39"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="23"/>
+      <c r="J33" s="22"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="39"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="35"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="22" t="s">
-        <v>42</v>
-      </c>
+      <c r="J34" s="20"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="39"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="35"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="23"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="39"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="23"/>
+      <c r="J36" s="22"/>
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1607,27 +1604,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Suma de señales hecha. Funciones ordenadas. Opciones personalizadas para grabacion de voz. Arreglado bug al borrar elementos de la lista (buffer) y reproducir. Espectograma funciona mejor.
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\yeyeye\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA4352C-50C1-4E7C-AF35-9140F4B3B8EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AC9C7F-BF0B-46BD-8F03-DB9D111FA72D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -596,6 +596,51 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -608,15 +653,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -624,48 +660,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -985,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,10 +996,10 @@
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="32"/>
+      <c r="H2" s="47"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1025,14 +1019,14 @@
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1044,14 +1038,14 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="41"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1061,14 +1055,14 @@
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="44"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1078,104 +1072,104 @@
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="47">
+      <c r="B9" s="40">
         <v>4</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="51" t="s">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="45"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="46"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="39"/>
     </row>
     <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="37"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="16"/>
     </row>
     <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="47">
+      <c r="B12" s="40">
         <v>6</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="51" t="s">
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="49"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="48"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="50"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="39"/>
     </row>
     <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
@@ -1185,14 +1179,14 @@
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
@@ -1202,14 +1196,14 @@
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
@@ -1219,14 +1213,14 @@
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1236,14 +1230,14 @@
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="13" t="s">
         <v>17</v>
       </c>
@@ -1253,14 +1247,14 @@
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
@@ -1270,14 +1264,14 @@
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="37"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1288,14 +1282,14 @@
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="35"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37"/>
       <c r="I21" s="13" t="s">
         <v>17</v>
       </c>
@@ -1305,14 +1299,14 @@
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
@@ -1324,14 +1318,14 @@
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="35"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
@@ -1341,14 +1335,14 @@
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="35"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
@@ -1360,14 +1354,14 @@
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="35"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
@@ -1377,14 +1371,14 @@
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
@@ -1394,14 +1388,14 @@
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="35"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
@@ -1411,14 +1405,14 @@
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="35"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
@@ -1428,14 +1422,14 @@
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="35"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
       <c r="I29" s="23" t="s">
         <v>30</v>
       </c>
@@ -1447,14 +1441,14 @@
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="35"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
@@ -1464,14 +1458,14 @@
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="35"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
@@ -1481,14 +1475,14 @@
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
@@ -1500,14 +1494,14 @@
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="33" t="s">
+      <c r="C33" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="35"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
@@ -1517,14 +1511,14 @@
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="35"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
@@ -1534,14 +1528,14 @@
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
@@ -1551,14 +1545,14 @@
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="35"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
@@ -1567,27 +1561,6 @@
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1604,6 +1577,27 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Filtros implementados. Mezcla de señales funciona correctamente. Solucionado error al montar los nombres en las variables aux
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\yeyeye\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AC9C7F-BF0B-46BD-8F03-DB9D111FA72D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF2EB1-146E-4F9E-ABD7-8FD0D95A9A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +196,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -514,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -566,9 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -581,21 +585,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -612,15 +640,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -641,27 +660,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Celda de comprobación" xfId="1" builtinId="23"/>
@@ -977,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K37"/>
+  <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,23 +996,23 @@
     <col min="9" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="47"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1015,18 +1023,18 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:10" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1034,193 +1042,194 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="16"/>
     </row>
-    <row r="8" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40">
+    <row r="9" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44">
         <v>4</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="42" t="s">
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="38"/>
-    </row>
-    <row r="10" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="39"/>
-    </row>
-    <row r="11" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="42"/>
+    </row>
+    <row r="10" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="45"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="37"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="40">
+      <c r="L11" s="51"/>
+    </row>
+    <row r="12" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="44">
         <v>6</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="42" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="38"/>
-    </row>
-    <row r="13" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="39"/>
-    </row>
-    <row r="14" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="42"/>
+    </row>
+    <row r="13" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="45"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="43"/>
+    </row>
+    <row r="14" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="50"/>
+    </row>
+    <row r="15" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" spans="2:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="25"/>
+    </row>
+    <row r="16" spans="2:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="27"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1230,14 +1239,14 @@
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
       <c r="I18" s="13" t="s">
         <v>17</v>
       </c>
@@ -1247,31 +1256,31 @@
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="28"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="32"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1282,14 +1291,14 @@
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="37"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
       <c r="I21" s="13" t="s">
         <v>17</v>
       </c>
@@ -1299,18 +1308,18 @@
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="37"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="48" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1318,35 +1327,35 @@
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="20"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="32"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="21" t="s">
+      <c r="J24" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1354,86 +1363,88 @@
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="37"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="20"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="20"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="22"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="32"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="24"/>
+      <c r="J28" s="49" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="23" t="s">
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1441,52 +1452,52 @@
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="25"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="32"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="22"/>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="32"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="21" t="s">
+      <c r="J32" s="20" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1494,73 +1505,94 @@
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="32"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="22"/>
+      <c r="J33" s="21"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="32"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="20"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="32"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="22"/>
+      <c r="J35" s="21"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="22"/>
+      <c r="J36" s="21"/>
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1577,27 +1609,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
eco y otros efectos añadidos
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Escritorio\FSI\Sonido\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877F75B4-D65A-4636-8684-31AA8B123BDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA21266-3A28-457B-9BAA-3844F01839B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -147,7 +147,7 @@
     <t>Número</t>
   </si>
   <si>
-    <t>David</t>
+    <t>CREO!!</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,12 +256,6 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -527,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -591,9 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -610,6 +601,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -674,9 +668,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -996,17 +987,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="10" width="19.44140625" customWidth="1"/>
+    <col min="9" max="10" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1032,7 +1023,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
@@ -1051,7 +1042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>1</v>
       </c>
@@ -1068,7 +1059,7 @@
       </c>
       <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
@@ -1085,7 +1076,7 @@
       </c>
       <c r="J7" s="16"/>
     </row>
-    <row r="8" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>3</v>
       </c>
@@ -1102,7 +1093,7 @@
       </c>
       <c r="J8" s="16"/>
     </row>
-    <row r="9" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="41">
         <v>4</v>
       </c>
@@ -1119,7 +1110,7 @@
       </c>
       <c r="J9" s="39"/>
     </row>
-    <row r="10" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="42"/>
       <c r="C10" s="30"/>
       <c r="D10" s="31"/>
@@ -1130,7 +1121,7 @@
       <c r="I10" s="44"/>
       <c r="J10" s="40"/>
     </row>
-    <row r="11" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
@@ -1146,9 +1137,9 @@
         <v>9</v>
       </c>
       <c r="J11" s="16"/>
-      <c r="L11" s="29"/>
-    </row>
-    <row r="12" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="28"/>
+    </row>
+    <row r="12" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41">
         <v>6</v>
       </c>
@@ -1165,7 +1156,7 @@
       </c>
       <c r="J12" s="39"/>
     </row>
-    <row r="13" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42"/>
       <c r="C13" s="30"/>
       <c r="D13" s="31"/>
@@ -1176,7 +1167,7 @@
       <c r="I13" s="44"/>
       <c r="J13" s="40"/>
     </row>
-    <row r="14" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
@@ -1191,9 +1182,9 @@
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
@@ -1208,9 +1199,9 @@
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="25"/>
-    </row>
-    <row r="16" spans="2:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="2:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>9</v>
       </c>
@@ -1225,9 +1216,9 @@
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="24"/>
-    </row>
-    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>10</v>
       </c>
@@ -1244,7 +1235,7 @@
       </c>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>11</v>
       </c>
@@ -1261,7 +1252,7 @@
       </c>
       <c r="J18" s="17"/>
     </row>
-    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>12</v>
       </c>
@@ -1276,9 +1267,9 @@
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="25"/>
-    </row>
-    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
@@ -1296,7 +1287,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>14</v>
       </c>
@@ -1313,7 +1304,7 @@
       </c>
       <c r="J21" s="18"/>
     </row>
-    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>15</v>
       </c>
@@ -1328,11 +1319,9 @@
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="25"/>
+    </row>
+    <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>16</v>
       </c>
@@ -1349,7 +1338,7 @@
       </c>
       <c r="J23" s="19"/>
     </row>
-    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
@@ -1364,11 +1353,9 @@
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>18</v>
       </c>
@@ -1385,7 +1372,7 @@
       </c>
       <c r="J25" s="19"/>
     </row>
-    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
@@ -1402,7 +1389,7 @@
       </c>
       <c r="J26" s="19"/>
     </row>
-    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
@@ -1419,7 +1406,7 @@
       </c>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
@@ -1434,11 +1421,9 @@
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
@@ -1453,11 +1438,9 @@
       <c r="I29" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10">
         <v>23</v>
       </c>
@@ -1472,9 +1455,11 @@
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="23"/>
-    </row>
-    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
@@ -1489,9 +1474,9 @@
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="21"/>
-    </row>
-    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
@@ -1506,11 +1491,9 @@
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J32" s="20"/>
+    </row>
+    <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>26</v>
       </c>
@@ -1527,7 +1510,7 @@
       </c>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
@@ -1544,7 +1527,7 @@
       </c>
       <c r="J34" s="19"/>
     </row>
-    <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
@@ -1561,7 +1544,7 @@
       </c>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
@@ -1578,7 +1561,7 @@
       </c>
       <c r="J36" s="21"/>
     </row>
-    <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
     <mergeCell ref="C5:H5"/>

</xml_diff>

<commit_message>
Añadido timestamp temporal al reproducir. Arreglado bug de mierda con el colorbar
</commit_message>
<xml_diff>
--- a/Funcionalidades.xlsx
+++ b/Funcionalidades.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Mario\Desktop\Programas_Teleco\proyectoSonido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Desktop\yeyeye\proyectoSonido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA21266-3A28-457B-9BAA-3844F01839B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D833550-8776-49FB-9352-63FA8669DA77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Funcionalidades del proyecto</t>
   </si>
@@ -147,7 +147,10 @@
     <t>Número</t>
   </si>
   <si>
-    <t>CREO!!</t>
+    <t>CREO!</t>
+  </si>
+  <si>
+    <t>Crees bien</t>
   </si>
 </sst>
 </file>
@@ -567,9 +570,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -604,6 +604,36 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -620,15 +650,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -649,26 +670,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -987,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,10 +1007,10 @@
       <c r="F2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="48"/>
+      <c r="H2" s="32"/>
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1027,14 +1030,14 @@
       <c r="B5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="47"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1046,14 +1049,14 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1063,14 +1066,14 @@
       <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="44"/>
       <c r="I7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1080,156 +1083,156 @@
       <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="16"/>
     </row>
     <row r="9" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="41">
+      <c r="B9" s="47">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="43" t="s">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="39"/>
+      <c r="J9" s="45"/>
     </row>
     <row r="10" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="42"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="40"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="46"/>
     </row>
     <row r="11" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>5</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
       <c r="I11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="J11" s="16"/>
-      <c r="L11" s="28"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41">
+      <c r="B12" s="47">
         <v>6</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="43" t="s">
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="39"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="42"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="40"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="46"/>
     </row>
     <row r="14" spans="2:12" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="26"/>
     </row>
     <row r="15" spans="2:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="38"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="24"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" spans="2:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>9</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="23"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>10</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
       <c r="I17" s="8" t="s">
         <v>17</v>
       </c>
@@ -1239,48 +1242,48 @@
       <c r="B18" s="10">
         <v>11</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
       <c r="I18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="17"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>12</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="24"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>13</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1291,279 +1294,303 @@
       <c r="B21" s="10">
         <v>14</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
       <c r="I21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="18"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>15</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="38"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
       <c r="I22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="25"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>16</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="38"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
       <c r="I23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="19"/>
+      <c r="J23" s="18"/>
     </row>
     <row r="24" spans="2:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10">
         <v>17</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="38"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10">
         <v>18</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="38"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
       <c r="I25" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="19"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10">
         <v>19</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
       <c r="I26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="19"/>
+      <c r="J26" s="18"/>
     </row>
     <row r="27" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <v>20</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
       <c r="I27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="21"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10">
         <v>21</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="38"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
       <c r="I28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="26"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>22</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="22" t="s">
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J29" s="18"/>
+      <c r="J29" s="17"/>
     </row>
     <row r="30" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10">
         <v>23</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="38"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="35"/>
       <c r="I30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="28" t="s">
         <v>40</v>
+      </c>
+      <c r="K30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10">
         <v>24</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="35"/>
       <c r="I31" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="19"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="2:11" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10">
         <v>25</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="38"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
       <c r="I32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="20"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>26</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
       <c r="I33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J33" s="21"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>27</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="38"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="35"/>
       <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J34" s="19"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>28</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="35"/>
       <c r="I35" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J35" s="21"/>
+      <c r="J35" s="20"/>
     </row>
     <row r="36" spans="2:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>29</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="38"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="21"/>
+      <c r="J36" s="20"/>
     </row>
     <row r="37" spans="2:10" ht="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C16:H16"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="C21:H21"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C35:H35"/>
@@ -1580,27 +1607,6 @@
     <mergeCell ref="C24:H24"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C16:H16"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="C19:H19"/>
-    <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I12:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>